<commit_message>
Flouro development completed! Testing left.
</commit_message>
<xml_diff>
--- a/ExcellDocs/ContentData.xlsx
+++ b/ExcellDocs/ContentData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goura\spring-workspace\FluoroFinderWeb\ExcellDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goura\spring-workspace\FluoroFinderWeb2\ExcellDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1450F13-C3C4-4860-8F56-E8632C884EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98D825A-3A0B-4B49-B88B-1B9B6BADE035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5172" yWindow="2100" windowWidth="10428" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InputData" sheetId="1" r:id="rId1"/>
@@ -485,7 +485,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
added explicit waits for main page loading
</commit_message>
<xml_diff>
--- a/ExcellDocs/ContentData.xlsx
+++ b/ExcellDocs/ContentData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goura\spring-workspace\ExcellAppFluoroFinder\ExcellDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6AAA99-B3FC-4CC1-BD79-3E361D6B7579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6F5A16-DC65-4639-81CB-526EF4D2649D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -485,7 +485,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -509,7 +509,7 @@
         <v>50316</v>
       </c>
       <c r="B2" s="2">
-        <v>50366</v>
+        <v>50616</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Increased script speed significantly
</commit_message>
<xml_diff>
--- a/ExcellDocs/ContentData.xlsx
+++ b/ExcellDocs/ContentData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goura\spring-workspace\ExcellAppFluoroFinder\ExcellDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A140A4E-ACBF-4681-ADDC-BE87E9042281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546BE84B-D3E7-4F7E-8FEA-8DD28ADBC57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -485,7 +485,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
some additional changes ikn test data
</commit_message>
<xml_diff>
--- a/ExcellDocs/ContentData.xlsx
+++ b/ExcellDocs/ContentData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goura\spring-workspace\ExcellAppFluoroFinder\ExcellDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546BE84B-D3E7-4F7E-8FEA-8DD28ADBC57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEAB2E1-7EB0-439E-A124-091E6A539B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -509,7 +509,7 @@
         <v>50316</v>
       </c>
       <c r="B2" s="2">
-        <v>50328</v>
+        <v>50415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code to add multiple execution result in the same excel File
</commit_message>
<xml_diff>
--- a/ExcellDocs/ContentData.xlsx
+++ b/ExcellDocs/ContentData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goura\spring-workspace\ExcellAppFluoroFinder\ExcellDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEAB2E1-7EB0-439E-A124-091E6A539B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9763E753-E1F8-41BC-BA07-A78A67147ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -485,7 +485,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -506,10 +506,10 @@
     </row>
     <row r="2" spans="1:2" ht="18.3" x14ac:dyDescent="0.7">
       <c r="A2" s="2">
-        <v>50316</v>
+        <v>50319</v>
       </c>
       <c r="B2" s="2">
-        <v>50415</v>
+        <v>50329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small change in DataDriven method to make it reusable
</commit_message>
<xml_diff>
--- a/ExcellDocs/ContentData.xlsx
+++ b/ExcellDocs/ContentData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goura\spring-workspace\ExcellAppFluoroFinder\ExcellDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9763E753-E1F8-41BC-BA07-A78A67147ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF326BF-8262-4E48-B45C-8BD1140F977E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -485,7 +485,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -506,10 +506,10 @@
     </row>
     <row r="2" spans="1:2" ht="18.3" x14ac:dyDescent="0.7">
       <c r="A2" s="2">
-        <v>50319</v>
+        <v>50316</v>
       </c>
       <c r="B2" s="2">
-        <v>50329</v>
+        <v>50318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>